<commit_message>
ADD: High parametrization and speedup for some dark reason :zap:
</commit_message>
<xml_diff>
--- a/data/best_solution.xlsx
+++ b/data/best_solution.xlsx
@@ -784,22 +784,22 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Mind Makers</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Geografia</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>História</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -812,27 +812,27 @@
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="M3" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
         </is>
       </c>
     </row>
@@ -842,27 +842,27 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
           <t>História</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Ed. Financeira</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="H4" s="4" t="n">
@@ -870,22 +870,22 @@
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>Música</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="L4" s="2" t="inlineStr">
-        <is>
-          <t>Ed. Financeira</t>
         </is>
       </c>
       <c r="M4" s="2" t="inlineStr">
@@ -900,27 +900,27 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>História</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
         </is>
       </c>
       <c r="H5" s="4" t="n">
@@ -928,27 +928,27 @@
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
-      <c r="L5" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
         </is>
       </c>
     </row>
@@ -1021,14 +1021,14 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
+          <t>Ciências</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Ciências</t>
-        </is>
-      </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Língua Portuguesa</t>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Educação Física</t>
         </is>
       </c>
       <c r="H7" s="4" t="n">
@@ -1049,22 +1049,22 @@
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="K7" s="2" t="inlineStr">
         <is>
-          <t>Ensino Religioso</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
-        </is>
-      </c>
-      <c r="M7" s="2" t="inlineStr">
-        <is>
-          <t>Música</t>
         </is>
       </c>
     </row>
@@ -1074,27 +1074,27 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Música</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Ciências</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Ciências</t>
+          <t>Ensino Religioso</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Ensino Religioso</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Mind Makers</t>
         </is>
       </c>
       <c r="H8" s="4" t="n">
@@ -1107,7 +1107,7 @@
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="L8" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Ensino Religioso</t>
         </is>
       </c>
       <c r="M8" s="2" t="inlineStr">
@@ -1270,27 +1270,27 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Música</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
           <t>Ed. Financeira</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
@@ -1298,27 +1298,27 @@
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="M13" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="J13" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>Ed. Financeira</t>
-        </is>
-      </c>
-      <c r="L13" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
-      <c r="M13" s="2" t="inlineStr">
-        <is>
-          <t>Artes</t>
         </is>
       </c>
     </row>
@@ -1328,27 +1328,27 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>Mind Makers</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
@@ -1356,27 +1356,27 @@
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="L14" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
         </is>
       </c>
-      <c r="J14" s="2" t="inlineStr">
+      <c r="M14" s="2" t="inlineStr">
         <is>
           <t>Matemática</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="L14" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
-      <c r="M14" s="2" t="inlineStr">
-        <is>
-          <t>Artes</t>
         </is>
       </c>
     </row>
@@ -1386,22 +1386,22 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>Geografia</t>
+          <t>História</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
@@ -1414,27 +1414,27 @@
       </c>
       <c r="I15" s="2" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>Música</t>
+        </is>
+      </c>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
         </is>
       </c>
-      <c r="J15" s="2" t="inlineStr">
+      <c r="M15" s="2" t="inlineStr">
         <is>
           <t>Matemática</t>
-        </is>
-      </c>
-      <c r="K15" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="L15" s="2" t="inlineStr">
-        <is>
-          <t>Mind Makers</t>
-        </is>
-      </c>
-      <c r="M15" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
         </is>
       </c>
     </row>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Ensino Religioso</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Artes</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
@@ -1535,22 +1535,22 @@
       </c>
       <c r="J17" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="K17" s="2" t="inlineStr">
+      <c r="L17" s="2" t="inlineStr">
+        <is>
+          <t>Ensino Religioso</t>
+        </is>
+      </c>
+      <c r="M17" s="2" t="inlineStr">
         <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="L17" s="2" t="inlineStr">
-        <is>
-          <t>Ensino Religioso</t>
-        </is>
-      </c>
-      <c r="M17" s="2" t="inlineStr">
-        <is>
-          <t>Educação Física</t>
         </is>
       </c>
     </row>
@@ -1565,14 +1565,14 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>Ensino Religioso</t>
-        </is>
-      </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
           <t>Ciências</t>
@@ -1580,7 +1580,7 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Artes</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
@@ -1593,22 +1593,22 @@
       </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="K18" s="2" t="inlineStr">
+      <c r="L18" s="2" t="inlineStr">
+        <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="M18" s="2" t="inlineStr">
         <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="L18" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="M18" s="2" t="inlineStr">
-        <is>
-          <t>Música</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
FEAT: fvck genalg heuristic and best solut in ~1min30s :fire:
</commit_message>
<xml_diff>
--- a/data/best_solution.xlsx
+++ b/data/best_solution.xlsx
@@ -784,27 +784,27 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
           <t>História</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
         </is>
       </c>
       <c r="H3" s="4" t="n">
@@ -812,12 +812,12 @@
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>História</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
@@ -827,12 +827,12 @@
       </c>
       <c r="L3" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Música</t>
         </is>
       </c>
     </row>
@@ -847,22 +847,22 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
           <t>História</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
         </is>
       </c>
       <c r="H4" s="4" t="n">
@@ -870,14 +870,14 @@
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
           <t>Artes</t>
         </is>
       </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>Música</t>
-        </is>
-      </c>
       <c r="K4" s="2" t="inlineStr">
         <is>
           <t>Inglês</t>
@@ -885,12 +885,12 @@
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Ed. Financeira</t>
         </is>
       </c>
       <c r="M4" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Inglês</t>
         </is>
       </c>
     </row>
@@ -910,17 +910,17 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="H5" s="4" t="n">
@@ -928,27 +928,27 @@
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
           <t>Artes</t>
         </is>
       </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>Ed. Financeira</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="M5" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Educação Física</t>
         </is>
       </c>
     </row>
@@ -1016,27 +1016,27 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
           <t>Artes</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>Educação Física</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="H7" s="4" t="n">
@@ -1049,22 +1049,22 @@
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>Ensino Religioso</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="K7" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
-      <c r="L7" s="2" t="inlineStr">
-        <is>
-          <t>Mind Makers</t>
-        </is>
-      </c>
       <c r="M7" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
     </row>
@@ -1074,27 +1074,27 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Ensino Religioso</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>Mind Makers</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="H8" s="4" t="n">
@@ -1107,22 +1107,22 @@
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="K8" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>Ensino Religioso</t>
-        </is>
-      </c>
       <c r="M8" s="2" t="inlineStr">
         <is>
-          <t>Educação Física</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
     </row>
@@ -1270,27 +1270,27 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>Música</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Inglês</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>Ed. Financeira</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
@@ -1298,27 +1298,27 @@
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
           <t>Geografia</t>
         </is>
       </c>
-      <c r="J13" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="L13" s="2" t="inlineStr">
+      <c r="M13" s="2" t="inlineStr">
         <is>
           <t>Matemática</t>
-        </is>
-      </c>
-      <c r="M13" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
         </is>
       </c>
     </row>
@@ -1328,27 +1328,27 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
-        </is>
-      </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
@@ -1356,22 +1356,22 @@
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
           <t>Geografia</t>
         </is>
       </c>
-      <c r="J14" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="M14" s="2" t="inlineStr">
@@ -1386,27 +1386,27 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>Educação Física</t>
         </is>
       </c>
       <c r="H15" s="4" t="n">
@@ -1419,17 +1419,17 @@
       </c>
       <c r="J15" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>História</t>
         </is>
       </c>
       <c r="K15" s="2" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="L15" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
         </is>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -1507,22 +1507,22 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Ciências</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
           <t>Ensino Religioso</t>
         </is>
       </c>
-      <c r="E17" s="2" t="inlineStr">
-        <is>
-          <t>Ciências</t>
-        </is>
-      </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Educação Física</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
@@ -1530,27 +1530,27 @@
       </c>
       <c r="I17" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="J17" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="J17" s="2" t="inlineStr">
-        <is>
-          <t>Artes</t>
-        </is>
-      </c>
       <c r="K17" s="2" t="inlineStr">
         <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="L17" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="L17" s="2" t="inlineStr">
-        <is>
-          <t>Ensino Religioso</t>
-        </is>
-      </c>
       <c r="M17" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Música</t>
         </is>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Ciências</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -1575,12 +1575,12 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Ciências</t>
+          <t>Mind Makers</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Música</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
@@ -1588,27 +1588,27 @@
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="J18" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="J18" s="2" t="inlineStr">
-        <is>
-          <t>Artes</t>
-        </is>
-      </c>
       <c r="K18" s="2" t="inlineStr">
         <is>
+          <t>Ensino Religioso</t>
+        </is>
+      </c>
+      <c r="L18" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="L18" s="2" t="inlineStr">
-        <is>
-          <t>Mind Makers</t>
-        </is>
-      </c>
       <c r="M18" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Educação Física</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add: creating objective var to direct search
</commit_message>
<xml_diff>
--- a/data/best_solution.xlsx
+++ b/data/best_solution.xlsx
@@ -784,22 +784,22 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
           <t>Geografia</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>Mind Makers</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -812,27 +812,27 @@
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>Matemática</t>
         </is>
       </c>
     </row>
@@ -842,27 +842,27 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Geografia</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
         </is>
       </c>
       <c r="H4" s="4" t="n">
@@ -870,7 +870,7 @@
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
@@ -885,12 +885,12 @@
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>Ed. Financeira</t>
+          <t>História</t>
         </is>
       </c>
       <c r="M4" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Matemática</t>
         </is>
       </c>
     </row>
@@ -905,22 +905,22 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>Ed. Financeira</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Inglês</t>
         </is>
       </c>
       <c r="H5" s="4" t="n">
@@ -938,17 +938,17 @@
       </c>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="M5" s="2" t="inlineStr">
-        <is>
-          <t>Educação Física</t>
         </is>
       </c>
     </row>
@@ -1016,27 +1016,27 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Ciências</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Artes</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Ciências</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
         </is>
       </c>
       <c r="H7" s="4" t="n">
@@ -1044,14 +1044,14 @@
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="J7" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
       <c r="K7" s="2" t="inlineStr">
         <is>
           <t>Ensino Religioso</t>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="M7" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Música</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Música</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Educação Física</t>
         </is>
       </c>
       <c r="H8" s="4" t="n">
@@ -1102,22 +1102,22 @@
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
+          <t>Matemática</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
           <t>Ciências</t>
         </is>
       </c>
-      <c r="J8" s="2" t="inlineStr">
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>Mind Makers</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
         <is>
           <t>Matemática</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="inlineStr">
-        <is>
-          <t>Mind Makers</t>
-        </is>
-      </c>
-      <c r="L8" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="M8" s="2" t="inlineStr">
@@ -1270,27 +1270,27 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
+          <t>Artes</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
           <t>Língua Portuguesa</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>Ed. Financeira</t>
-        </is>
-      </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Mind Makers</t>
         </is>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Artes</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
@@ -1298,27 +1298,27 @@
       </c>
       <c r="I13" s="2" t="inlineStr">
         <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
         </is>
       </c>
-      <c r="J13" s="2" t="inlineStr">
+      <c r="M13" s="2" t="inlineStr">
         <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>Mind Makers</t>
-        </is>
-      </c>
-      <c r="L13" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
-      <c r="M13" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
         </is>
       </c>
     </row>
@@ -1328,27 +1328,27 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>História</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>Matemática</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
-        </is>
-      </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Música</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
@@ -1356,27 +1356,27 @@
       </c>
       <c r="I14" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>Inglês</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
         </is>
       </c>
-      <c r="J14" s="2" t="inlineStr">
-        <is>
-          <t>História</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
       <c r="L14" s="2" t="inlineStr">
         <is>
-          <t>Inglês</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="M14" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
     </row>
@@ -1386,27 +1386,27 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Matemática</t>
+          <t>Inglês</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
+          <t>Ed. Financeira</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
           <t>História</t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
-        <is>
-          <t>Geografia</t>
-        </is>
-      </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>Língua Portuguesa</t>
+          <t>Educação Física</t>
         </is>
       </c>
       <c r="H15" s="4" t="n">
@@ -1419,17 +1419,17 @@
       </c>
       <c r="J15" s="2" t="inlineStr">
         <is>
-          <t>História</t>
+          <t>Geografia</t>
         </is>
       </c>
       <c r="K15" s="2" t="inlineStr">
         <is>
+          <t>Língua Portuguesa</t>
+        </is>
+      </c>
+      <c r="L15" s="2" t="inlineStr">
+        <is>
           <t>Inglês</t>
-        </is>
-      </c>
-      <c r="L15" s="2" t="inlineStr">
-        <is>
-          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="M15" s="2" t="inlineStr">
@@ -1502,14 +1502,14 @@
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
+          <t>Ciências</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
         </is>
       </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>Ciências</t>
-        </is>
-      </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
           <t>Língua Portuguesa</t>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>Educação Física</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="K17" s="2" t="inlineStr">
         <is>
-          <t>Ed. Financeira</t>
+          <t>Mind Makers</t>
         </is>
       </c>
       <c r="L17" s="2" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="M17" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>Educação Física</t>
         </is>
       </c>
     </row>
@@ -1560,14 +1560,14 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
+          <t>Ciências</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
           <t>Matemática</t>
         </is>
       </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>Ciências</t>
-        </is>
-      </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
           <t>Língua Portuguesa</t>
@@ -1575,12 +1575,12 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Mind Makers</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>Música</t>
+          <t>Matemática</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="I18" s="2" t="inlineStr">
         <is>
-          <t>Artes</t>
+          <t>Língua Portuguesa</t>
         </is>
       </c>
       <c r="J18" s="2" t="inlineStr">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="M18" s="2" t="inlineStr">
         <is>
-          <t>Educação Física</t>
+          <t>Música</t>
         </is>
       </c>
     </row>

</xml_diff>